<commit_message>
analysis of cluster movement
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/vector of movement-2.xlsx
+++ b/migforecasting/clustering/vector of movement-2.xlsx
@@ -546,11 +546,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>